<commit_message>
update code review file
</commit_message>
<xml_diff>
--- a/代码检视.xlsx
+++ b/代码检视.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>检视问题</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>解决</t>
-  </si>
-  <si>
-    <t>是否修改</t>
   </si>
   <si>
     <t>首页宽度变小，头部部分的搜索会遮挡其他
@@ -52,6 +49,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>样式对宽度小于</t>
     </r>
@@ -71,6 +69,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>的支持不够全面</t>
     </r>
@@ -82,6 +81,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>重新编写宽度小于</t>
     </r>
@@ -101,6 +101,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>的样式</t>
     </r>
@@ -118,6 +119,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>内容部分</t>
     </r>
@@ -137,6 +139,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>上方内边距不够</t>
     </r>
@@ -148,6 +151,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>设置宽度小于</t>
     </r>
@@ -167,6 +171,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>下内容部分</t>
     </r>
@@ -186,6 +191,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>上方内边距</t>
     </r>
@@ -209,6 +215,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>样式文件</t>
     </r>
@@ -228,6 +235,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>、</t>
     </r>
@@ -247,6 +255,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>合并</t>
     </r>
@@ -261,6 +270,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>合并</t>
     </r>
@@ -280,6 +290,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>和</t>
     </r>
@@ -299,6 +310,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>目录下样式文件</t>
     </r>
@@ -320,6 +332,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>重用</t>
     </r>
@@ -339,6 +352,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>文件</t>
     </r>
@@ -360,6 +374,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>执行一次</t>
     </r>
@@ -381,6 +396,7 @@
         <color rgb="FF000000"/>
         <rFont val="文泉驿点阵正黑"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t>行</t>
     </r>
@@ -405,6 +421,7 @@
       <color rgb="FF000000"/>
       <name val="文泉驿点阵正黑"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -597,19 +614,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.6351931330472"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5579399141631"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.0257510729614"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9570815450644"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.54077253218884"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.0171673819742"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.2317596566524"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.8412017167382"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.3991416309013"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.2188841201717"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -625,98 +642,88 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="44" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="36" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="50" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="4"/>
     </row>
-    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -742,7 +749,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.54077253218884"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2188841201717"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -768,7 +775,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.54077253218884"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2188841201717"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
fix search and toc style
</commit_message>
<xml_diff>
--- a/代码检视.xlsx
+++ b/代码检视.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
   <si>
     <t>检视时间</t>
   </si>
@@ -549,7 +549,7 @@
     <t>搜索范围有控制，只能搜索html文件，而那些不需要输入完整路径也可以访问的页面就被排除在外了</t>
   </si>
   <si>
-    <t>修改搜索范围,只排除xml和json文件，并以头信息的“search: exclude”区分是否在搜索范围内</t>
+    <t>修改搜索范围,以头信息的“search: exclude”区分是否在搜索范围内</t>
   </si>
   <si>
     <t>搜索结果重复</t>
@@ -568,6 +568,18 @@
   </si>
   <si>
     <t>引入需要的样式文件</t>
+  </si>
+  <si>
+    <t>独立搜索页面样式和整体样式不符</t>
+  </si>
+  <si>
+    <t>修改搜索页面样式</t>
+  </si>
+  <si>
+    <t>头部搜索弹出框被目录遮挡</t>
+  </si>
+  <si>
+    <t>右侧目录高度未与文本平齐</t>
   </si>
 </sst>
 </file>
@@ -740,8 +752,8 @@
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1297,11 +1309,17 @@
         <v>42887</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="H22" s="2" t="n">
         <v>42887</v>
       </c>
@@ -1314,7 +1332,9 @@
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1330,7 +1350,9 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>81</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>

</xml_diff>